<commit_message>
Ultima actualización del CV
</commit_message>
<xml_diff>
--- a/CV_Díaz_Juan/info_cv - copia.xlsx
+++ b/CV_Díaz_Juan/info_cv - copia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Documents\CV\CV_Díaz_Juan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58094DDE-9A19-4876-BBD1-5252CBA8DA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA5A6DB-B49D-4622-8949-02F00D6D3BCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{34DB0F05-D7C4-422F-BAAA-B0A980F53D90}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
   <si>
     <t>Grado</t>
   </si>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t>Manejo de grupos, diseño de tareas de evaluación, generación de materiales educativos y planificación de actividades</t>
-  </si>
-  <si>
-    <t>Ponente</t>
   </si>
 </sst>
 </file>
@@ -178,7 +175,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -186,7 +183,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -558,10 +554,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F839D54-E766-4C3B-8340-6749AD15D5EB}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,7 +596,7 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -636,11 +632,6 @@
       </c>
       <c r="E4" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>